<commit_message>
Move existing CoV Bundle to dev and add new test OCABundle
Signed-off-by: Stephen Curran <swcurran@gmail.com>
</commit_message>
<xml_diff>
--- a/OCABundles/schema/CityOfVancouver/test-property-rental-business-licence/municipal-property-rental-business-licence-OCA.xlsx
+++ b/OCABundles/schema/CityOfVancouver/test-property-rental-business-licence/municipal-property-rental-business-licence-OCA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathieuglaude/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1281A0A-4977-6644-B322-D59329634412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75E173E3-5593-884B-8FCD-A1653C42ADD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Start Here" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="221">
   <si>
     <t>OCA DATA CAPTURE SPECIFICATION</t>
   </si>
@@ -1494,9 +1494,6 @@
     <t>watermark</t>
   </si>
   <si>
-    <t>DEMONSTRATION</t>
-  </si>
-  <si>
     <t>The issued date of the business licence.</t>
   </si>
   <si>
@@ -1704,7 +1701,7 @@
     <t>The date on which the business is permitted to begin operating under the issued licence.</t>
   </si>
   <si>
-    <t>City of Vancouver (DEV)</t>
+    <t>City of Vancouver (UAT)</t>
   </si>
 </sst>
 </file>
@@ -1879,7 +1876,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1938,12 +1935,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFECECEC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2626,14 +2617,14 @@
     <xf numFmtId="0" fontId="18" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2675,22 +2666,22 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4923,8 +4914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="12.75" customHeight="1"/>
@@ -5335,20 +5326,20 @@
     </row>
     <row r="12" spans="1:27" ht="12.75" customHeight="1">
       <c r="A12" s="47"/>
-      <c r="B12" s="94" t="s">
-        <v>218</v>
-      </c>
-      <c r="C12" s="95" t="s">
+      <c r="B12" s="91" t="s">
+        <v>217</v>
+      </c>
+      <c r="C12" s="92" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="96"/>
-      <c r="E12" s="97" t="s">
+      <c r="D12" s="93"/>
+      <c r="E12" s="94" t="s">
         <v>101</v>
       </c>
-      <c r="F12" s="96" t="s">
+      <c r="F12" s="93" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="96" t="s">
+      <c r="G12" s="93" t="s">
         <v>111</v>
       </c>
       <c r="H12" s="47"/>
@@ -5420,7 +5411,7 @@
         <v/>
       </c>
       <c r="B14" s="56" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C14" s="54" t="s">
         <v>65</v>
@@ -5762,7 +5753,7 @@
         <v/>
       </c>
       <c r="B23" s="56" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C23" s="54" t="s">
         <v>65</v>
@@ -5800,7 +5791,7 @@
         <v/>
       </c>
       <c r="B24" s="56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C24" s="54" t="s">
         <v>65</v>
@@ -5952,7 +5943,7 @@
         <v/>
       </c>
       <c r="B28" s="56" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C28" s="54" t="s">
         <v>67</v>
@@ -6103,8 +6094,8 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B32" s="73" t="s">
-        <v>179</v>
+      <c r="B32" s="72" t="s">
+        <v>178</v>
       </c>
       <c r="C32" s="54" t="s">
         <v>65</v>
@@ -6141,8 +6132,8 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B33" s="73" t="s">
-        <v>180</v>
+      <c r="B33" s="72" t="s">
+        <v>179</v>
       </c>
       <c r="C33" s="54" t="s">
         <v>65</v>
@@ -6179,8 +6170,8 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B34" s="73" t="s">
-        <v>181</v>
+      <c r="B34" s="72" t="s">
+        <v>180</v>
       </c>
       <c r="C34" s="54" t="s">
         <v>65</v>
@@ -6217,8 +6208,8 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B35" s="73" t="s">
-        <v>182</v>
+      <c r="B35" s="72" t="s">
+        <v>181</v>
       </c>
       <c r="C35" s="54" t="s">
         <v>65</v>
@@ -6255,8 +6246,8 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B36" s="73" t="s">
-        <v>183</v>
+      <c r="B36" s="72" t="s">
+        <v>182</v>
       </c>
       <c r="C36" s="54" t="s">
         <v>65</v>
@@ -6293,8 +6284,8 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B37" s="73" t="s">
-        <v>184</v>
+      <c r="B37" s="72" t="s">
+        <v>183</v>
       </c>
       <c r="C37" s="54" t="s">
         <v>65</v>
@@ -37294,10 +37285,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="expression" dxfId="1" priority="39">
+    <cfRule type="expression" dxfId="5" priority="39">
       <formula>AND(ISBLANK(B11),NOT(SUMPRODUCT(C11:AA11&lt;&gt;"")=0))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="40">
+    <cfRule type="expression" dxfId="4" priority="40">
       <formula>AND(ISBLANK(B11), SUMPRODUCT(MAX((B11:B1012&lt;&gt;"")*ROW(B11:B1012))) &gt; 0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -37332,8 +37323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="12.75" customHeight="1"/>
@@ -37386,18 +37377,18 @@
         <v>130</v>
       </c>
       <c r="B4" s="63" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C4" s="64" t="str">
         <f>IF(ISBLANK(Main!$B4),"",Main!$B4)</f>
         <v>business_licence_type</v>
       </c>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="74" t="s">
         <v>131</v>
       </c>
       <c r="E4" s="65"/>
-      <c r="F4" s="75" t="s">
-        <v>199</v>
+      <c r="F4" s="74" t="s">
+        <v>198</v>
       </c>
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
@@ -37431,11 +37422,11 @@
         <f>IF(ISBLANK(Main!$B5),"",Main!$B5)</f>
         <v>business_sub_type</v>
       </c>
-      <c r="D5" s="74" t="s">
-        <v>185</v>
+      <c r="D5" s="73" t="s">
+        <v>184</v>
       </c>
       <c r="E5" s="68"/>
-      <c r="F5" s="75" t="s">
+      <c r="F5" s="74" t="s">
         <v>134</v>
       </c>
       <c r="G5" s="26"/>
@@ -37463,18 +37454,18 @@
       <c r="A6" s="66" t="s">
         <v>135</v>
       </c>
-      <c r="B6" s="91" t="s">
-        <v>221</v>
+      <c r="B6" s="75" t="s">
+        <v>220</v>
       </c>
       <c r="C6" s="47" t="str">
         <f>IF(ISBLANK(Main!$B6),"",Main!$B6)</f>
         <v>business_trade_name</v>
       </c>
-      <c r="D6" s="74" t="s">
+      <c r="D6" s="73" t="s">
         <v>137</v>
       </c>
       <c r="E6" s="68"/>
-      <c r="F6" s="75" t="s">
+      <c r="F6" s="74" t="s">
         <v>138</v>
       </c>
       <c r="G6" s="26"/>
@@ -37509,11 +37500,11 @@
         <f>IF(ISBLANK(Main!$B7),"",Main!$B7)</f>
         <v>licence_number</v>
       </c>
-      <c r="D7" s="74" t="s">
+      <c r="D7" s="73" t="s">
         <v>140</v>
       </c>
       <c r="E7" s="68"/>
-      <c r="F7" s="75" t="s">
+      <c r="F7" s="74" t="s">
         <v>141</v>
       </c>
       <c r="G7" s="26"/>
@@ -37548,11 +37539,11 @@
         <f>IF(ISBLANK(Main!$B8),"",Main!$B8)</f>
         <v>licence_revision_number</v>
       </c>
-      <c r="D8" s="74" t="s">
+      <c r="D8" s="73" t="s">
         <v>144</v>
       </c>
       <c r="E8" s="68"/>
-      <c r="F8" s="75" t="s">
+      <c r="F8" s="74" t="s">
         <v>145</v>
       </c>
       <c r="G8" s="26"/>
@@ -37585,11 +37576,11 @@
         <f>IF(ISBLANK(Main!$B9),"",Main!$B9)</f>
         <v>licence_holder_given_name</v>
       </c>
-      <c r="D9" s="74" t="s">
-        <v>186</v>
+      <c r="D9" s="73" t="s">
+        <v>185</v>
       </c>
       <c r="E9" s="68"/>
-      <c r="F9" s="75" t="s">
+      <c r="F9" s="74" t="s">
         <v>147</v>
       </c>
       <c r="G9" s="26"/>
@@ -37624,11 +37615,11 @@
         <f>IF(ISBLANK(Main!$B10),"",Main!$B10)</f>
         <v>licence_holder_family_name</v>
       </c>
-      <c r="D10" s="74" t="s">
-        <v>187</v>
+      <c r="D10" s="73" t="s">
+        <v>186</v>
       </c>
       <c r="E10" s="68"/>
-      <c r="F10" s="75" t="s">
+      <c r="F10" s="74" t="s">
         <v>149</v>
       </c>
       <c r="G10" s="26"/>
@@ -37656,19 +37647,17 @@
       <c r="A11" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="B11" s="72" t="s">
-        <v>151</v>
-      </c>
+      <c r="B11" s="97"/>
       <c r="C11" s="47" t="str">
         <f>IF(ISBLANK(Main!$B11),"",Main!$B11)</f>
         <v>licence_issued_dateint</v>
       </c>
-      <c r="D11" s="74" t="s">
-        <v>188</v>
+      <c r="D11" s="73" t="s">
+        <v>187</v>
       </c>
       <c r="E11" s="68"/>
-      <c r="F11" s="75" t="s">
-        <v>152</v>
+      <c r="F11" s="74" t="s">
+        <v>151</v>
       </c>
       <c r="G11" s="26"/>
       <c r="H11" s="26"/>
@@ -37694,15 +37683,15 @@
     <row r="12" spans="1:26" ht="12.75" customHeight="1">
       <c r="A12" s="66"/>
       <c r="B12" s="70"/>
-      <c r="C12" s="92" t="s">
+      <c r="C12" s="95" t="s">
+        <v>217</v>
+      </c>
+      <c r="D12" s="95" t="s">
         <v>218</v>
       </c>
-      <c r="D12" s="92" t="s">
+      <c r="E12" s="96"/>
+      <c r="F12" s="95" t="s">
         <v>219</v>
-      </c>
-      <c r="E12" s="93"/>
-      <c r="F12" s="92" t="s">
-        <v>220</v>
       </c>
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
@@ -37732,12 +37721,12 @@
         <f>IF(ISBLANK(Main!$B13),"",Main!$B13)</f>
         <v>licence_expiry_dateint</v>
       </c>
-      <c r="D13" s="74" t="s">
-        <v>189</v>
+      <c r="D13" s="73" t="s">
+        <v>188</v>
       </c>
       <c r="E13" s="68"/>
-      <c r="F13" s="75" t="s">
-        <v>153</v>
+      <c r="F13" s="74" t="s">
+        <v>152</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="26"/>
@@ -37767,12 +37756,12 @@
         <f>IF(ISBLANK(Main!$B14),"",Main!$B14)</f>
         <v>unit</v>
       </c>
-      <c r="D14" s="74" t="s">
+      <c r="D14" s="73" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14" s="68"/>
+      <c r="F14" s="74" t="s">
         <v>154</v>
-      </c>
-      <c r="E14" s="68"/>
-      <c r="F14" s="75" t="s">
-        <v>155</v>
       </c>
       <c r="G14" s="26"/>
       <c r="H14" s="26"/>
@@ -37802,12 +37791,12 @@
         <f>IF(ISBLANK(Main!$B15),"",Main!$B15)</f>
         <v>unit_type</v>
       </c>
-      <c r="D15" s="74" t="s">
+      <c r="D15" s="73" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="68"/>
+      <c r="F15" s="74" t="s">
         <v>156</v>
-      </c>
-      <c r="E15" s="68"/>
-      <c r="F15" s="75" t="s">
-        <v>157</v>
       </c>
       <c r="G15" s="26"/>
       <c r="H15" s="26"/>
@@ -37837,12 +37826,12 @@
         <f>IF(ISBLANK(Main!$B16),"",Main!$B16)</f>
         <v>street_number</v>
       </c>
-      <c r="D16" s="74" t="s">
+      <c r="D16" s="73" t="s">
+        <v>157</v>
+      </c>
+      <c r="E16" s="68"/>
+      <c r="F16" s="74" t="s">
         <v>158</v>
-      </c>
-      <c r="E16" s="68"/>
-      <c r="F16" s="75" t="s">
-        <v>159</v>
       </c>
       <c r="G16" s="26"/>
       <c r="H16" s="26"/>
@@ -37872,12 +37861,12 @@
         <f>IF(ISBLANK(Main!$B17),"",Main!$B17)</f>
         <v>street_name</v>
       </c>
-      <c r="D17" s="74" t="s">
+      <c r="D17" s="73" t="s">
+        <v>159</v>
+      </c>
+      <c r="E17" s="68"/>
+      <c r="F17" s="74" t="s">
         <v>160</v>
-      </c>
-      <c r="E17" s="68"/>
-      <c r="F17" s="75" t="s">
-        <v>161</v>
       </c>
       <c r="G17" s="26"/>
       <c r="H17" s="26"/>
@@ -37907,12 +37896,12 @@
         <f>IF(ISBLANK(Main!$B18),"",Main!$B18)</f>
         <v>municipality</v>
       </c>
-      <c r="D18" s="74" t="s">
+      <c r="D18" s="73" t="s">
+        <v>161</v>
+      </c>
+      <c r="E18" s="68"/>
+      <c r="F18" s="74" t="s">
         <v>162</v>
-      </c>
-      <c r="E18" s="68"/>
-      <c r="F18" s="75" t="s">
-        <v>163</v>
       </c>
       <c r="G18" s="26"/>
       <c r="H18" s="26"/>
@@ -37942,12 +37931,12 @@
         <f>IF(ISBLANK(Main!$B19),"",Main!$B19)</f>
         <v>municipality_status</v>
       </c>
-      <c r="D19" s="74" t="s">
-        <v>190</v>
+      <c r="D19" s="73" t="s">
+        <v>189</v>
       </c>
       <c r="E19" s="68"/>
-      <c r="F19" s="75" t="s">
-        <v>200</v>
+      <c r="F19" s="74" t="s">
+        <v>199</v>
       </c>
       <c r="G19" s="26"/>
       <c r="H19" s="26"/>
@@ -37977,12 +37966,12 @@
         <f>IF(ISBLANK(Main!$B20),"",Main!$B20)</f>
         <v>regional_district</v>
       </c>
-      <c r="D20" s="74" t="s">
-        <v>164</v>
+      <c r="D20" s="73" t="s">
+        <v>163</v>
       </c>
       <c r="E20" s="68"/>
-      <c r="F20" s="75" t="s">
-        <v>201</v>
+      <c r="F20" s="74" t="s">
+        <v>200</v>
       </c>
       <c r="G20" s="26"/>
       <c r="H20" s="26"/>
@@ -38012,12 +38001,12 @@
         <f>IF(ISBLANK(Main!$B21),"",Main!$B21)</f>
         <v>province_territory</v>
       </c>
-      <c r="D21" s="74" t="s">
-        <v>165</v>
+      <c r="D21" s="73" t="s">
+        <v>164</v>
       </c>
       <c r="E21" s="68"/>
-      <c r="F21" s="75" t="s">
-        <v>202</v>
+      <c r="F21" s="74" t="s">
+        <v>201</v>
       </c>
       <c r="G21" s="26"/>
       <c r="H21" s="26"/>
@@ -38047,12 +38036,12 @@
         <f>IF(ISBLANK(Main!$B22),"",Main!$B22)</f>
         <v>postal_code</v>
       </c>
-      <c r="D22" s="74" t="s">
+      <c r="D22" s="73" t="s">
+        <v>165</v>
+      </c>
+      <c r="E22" s="68"/>
+      <c r="F22" s="74" t="s">
         <v>166</v>
-      </c>
-      <c r="E22" s="68"/>
-      <c r="F22" s="75" t="s">
-        <v>167</v>
       </c>
       <c r="G22" s="26"/>
       <c r="H22" s="26"/>
@@ -38082,12 +38071,12 @@
         <f>IF(ISBLANK(Main!$B23),"",Main!$B23)</f>
         <v>country</v>
       </c>
-      <c r="D23" s="74" t="s">
+      <c r="D23" s="73" t="s">
         <v>121</v>
       </c>
       <c r="E23" s="68"/>
-      <c r="F23" s="75" t="s">
-        <v>168</v>
+      <c r="F23" s="74" t="s">
+        <v>167</v>
       </c>
       <c r="G23" s="26"/>
       <c r="H23" s="26"/>
@@ -38117,12 +38106,12 @@
         <f>IF(ISBLANK(Main!$B24),"",Main!$B24)</f>
         <v>full_licence_address</v>
       </c>
-      <c r="D24" s="74" t="s">
-        <v>191</v>
+      <c r="D24" s="73" t="s">
+        <v>190</v>
       </c>
       <c r="E24" s="68"/>
-      <c r="F24" s="75" t="s">
-        <v>203</v>
+      <c r="F24" s="74" t="s">
+        <v>202</v>
       </c>
       <c r="G24" s="26"/>
       <c r="H24" s="26"/>
@@ -38152,12 +38141,12 @@
         <f>IF(ISBLANK(Main!$B25),"",Main!$B25)</f>
         <v>property_residence_type</v>
       </c>
-      <c r="D25" s="74" t="s">
-        <v>169</v>
+      <c r="D25" s="73" t="s">
+        <v>168</v>
       </c>
       <c r="E25" s="47"/>
-      <c r="F25" s="75" t="s">
-        <v>204</v>
+      <c r="F25" s="74" t="s">
+        <v>203</v>
       </c>
       <c r="G25" s="26"/>
       <c r="H25" s="26"/>
@@ -38187,12 +38176,12 @@
         <f>IF(ISBLANK(Main!$B26),"",Main!$B26)</f>
         <v>local_area</v>
       </c>
-      <c r="D26" s="74" t="s">
-        <v>170</v>
+      <c r="D26" s="73" t="s">
+        <v>169</v>
       </c>
       <c r="E26" s="47"/>
-      <c r="F26" s="75" t="s">
-        <v>205</v>
+      <c r="F26" s="74" t="s">
+        <v>204</v>
       </c>
       <c r="G26" s="26"/>
       <c r="H26" s="26"/>
@@ -38222,12 +38211,12 @@
         <f>IF(ISBLANK(Main!$B27),"",Main!$B27)</f>
         <v>location_type</v>
       </c>
-      <c r="D27" s="74" t="s">
-        <v>171</v>
+      <c r="D27" s="73" t="s">
+        <v>170</v>
       </c>
       <c r="E27" s="47"/>
-      <c r="F27" s="75" t="s">
-        <v>206</v>
+      <c r="F27" s="74" t="s">
+        <v>205</v>
       </c>
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
@@ -38257,12 +38246,12 @@
         <f>IF(ISBLANK(Main!$B28),"",Main!$B28)</f>
         <v>number_of_dwelling_unitsint</v>
       </c>
-      <c r="D28" s="74" t="s">
-        <v>172</v>
+      <c r="D28" s="73" t="s">
+        <v>171</v>
       </c>
       <c r="E28" s="47"/>
-      <c r="F28" s="75" t="s">
-        <v>207</v>
+      <c r="F28" s="74" t="s">
+        <v>206</v>
       </c>
       <c r="G28" s="26"/>
       <c r="H28" s="26"/>
@@ -38292,12 +38281,12 @@
         <f>IF(ISBLANK(Main!$B29),"",Main!$B29)</f>
         <v>PID</v>
       </c>
-      <c r="D29" s="74" t="s">
-        <v>173</v>
+      <c r="D29" s="73" t="s">
+        <v>172</v>
       </c>
       <c r="E29" s="47"/>
-      <c r="F29" s="75" t="s">
-        <v>208</v>
+      <c r="F29" s="74" t="s">
+        <v>207</v>
       </c>
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
@@ -38327,12 +38316,12 @@
         <f>IF(ISBLANK(Main!$B30),"",Main!$B30)</f>
         <v>strata_flag</v>
       </c>
-      <c r="D30" s="74" t="s">
-        <v>192</v>
+      <c r="D30" s="73" t="s">
+        <v>191</v>
       </c>
       <c r="E30" s="47"/>
-      <c r="F30" s="75" t="s">
-        <v>209</v>
+      <c r="F30" s="74" t="s">
+        <v>208</v>
       </c>
       <c r="G30" s="26"/>
       <c r="H30" s="26"/>
@@ -38362,12 +38351,12 @@
         <f>IF(ISBLANK(Main!$B31),"",Main!$B31)</f>
         <v>GIS_coordinates</v>
       </c>
-      <c r="D31" s="74" t="s">
-        <v>174</v>
+      <c r="D31" s="73" t="s">
+        <v>173</v>
       </c>
       <c r="E31" s="47"/>
-      <c r="F31" s="75" t="s">
-        <v>210</v>
+      <c r="F31" s="74" t="s">
+        <v>209</v>
       </c>
       <c r="G31" s="26"/>
       <c r="H31" s="26"/>
@@ -38397,12 +38386,12 @@
         <f>IF(ISBLANK(Main!$B32),"",Main!$B32)</f>
         <v>identity_verification_proof</v>
       </c>
-      <c r="D32" s="74" t="s">
-        <v>193</v>
+      <c r="D32" s="73" t="s">
+        <v>192</v>
       </c>
       <c r="E32" s="47"/>
-      <c r="F32" s="75" t="s">
-        <v>211</v>
+      <c r="F32" s="74" t="s">
+        <v>210</v>
       </c>
       <c r="G32" s="26"/>
       <c r="H32" s="26"/>
@@ -38432,12 +38421,12 @@
         <f>IF(ISBLANK(Main!$B33),"",Main!$B33)</f>
         <v>primary_address_verification_proof</v>
       </c>
-      <c r="D33" s="74" t="s">
-        <v>194</v>
+      <c r="D33" s="73" t="s">
+        <v>193</v>
       </c>
       <c r="E33" s="47"/>
-      <c r="F33" s="75" t="s">
-        <v>212</v>
+      <c r="F33" s="74" t="s">
+        <v>211</v>
       </c>
       <c r="G33" s="26"/>
       <c r="H33" s="26"/>
@@ -38467,12 +38456,12 @@
         <f>IF(ISBLANK(Main!$B34),"",Main!$B34)</f>
         <v>property_owner_proof</v>
       </c>
-      <c r="D34" s="74" t="s">
-        <v>195</v>
+      <c r="D34" s="73" t="s">
+        <v>194</v>
       </c>
       <c r="E34" s="47"/>
-      <c r="F34" s="75" t="s">
-        <v>213</v>
+      <c r="F34" s="74" t="s">
+        <v>212</v>
       </c>
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
@@ -38502,12 +38491,12 @@
         <f>IF(ISBLANK(Main!$B35),"",Main!$B35)</f>
         <v>authorized_verification_proof</v>
       </c>
-      <c r="D35" s="74" t="s">
-        <v>196</v>
+      <c r="D35" s="73" t="s">
+        <v>195</v>
       </c>
       <c r="E35" s="47"/>
-      <c r="F35" s="75" t="s">
-        <v>214</v>
+      <c r="F35" s="74" t="s">
+        <v>213</v>
       </c>
       <c r="G35" s="26"/>
       <c r="H35" s="26"/>
@@ -38537,12 +38526,12 @@
         <f>IF(ISBLANK(Main!$B36),"",Main!$B36)</f>
         <v>licence_summary</v>
       </c>
-      <c r="D36" s="74" t="s">
-        <v>197</v>
+      <c r="D36" s="73" t="s">
+        <v>196</v>
       </c>
       <c r="E36" s="47"/>
-      <c r="F36" s="75" t="s">
-        <v>215</v>
+      <c r="F36" s="74" t="s">
+        <v>214</v>
       </c>
       <c r="G36" s="26"/>
       <c r="H36" s="26"/>
@@ -38572,12 +38561,12 @@
         <f>IF(ISBLANK(Main!$B37),"",Main!$B37)</f>
         <v>short_address</v>
       </c>
-      <c r="D37" s="74" t="s">
-        <v>198</v>
+      <c r="D37" s="73" t="s">
+        <v>197</v>
       </c>
       <c r="E37" s="47"/>
-      <c r="F37" s="75" t="s">
-        <v>216</v>
+      <c r="F37" s="74" t="s">
+        <v>215</v>
       </c>
       <c r="G37" s="26"/>
       <c r="H37" s="26"/>
@@ -68548,22 +68537,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:F11 E13:F16 D38:F1003 E33:F37 E17:E32">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND(NOT(ISBLANK(D4)),$C4="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17:F31">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND(NOT(ISBLANK(F17)),$C18="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D11 D14:D37">
-    <cfRule type="expression" dxfId="3" priority="27">
+    <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(NOT(ISBLANK(D5)),$C4="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="2" priority="36">
+    <cfRule type="expression" dxfId="0" priority="36">
       <formula>AND(NOT(ISBLANK(D13)),$C11="")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>